<commit_message>
Splitted project into 5 parts
</commit_message>
<xml_diff>
--- a/machine-learning/sentiment-analysis-with-python/outputs/TECHNICAL.xlsx
+++ b/machine-learning/sentiment-analysis-with-python/outputs/TECHNICAL.xlsx
@@ -1,21 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06af25a4dc2b6874/Documents/Portfolio/machine-learning/sentiment-analysis-with-python/outputs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_5EA96176752833A54E39BD3C5170DECC3C6264CD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CE289E5-E1D0-42F4-9F6F-C312CA298E9E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PARAMETERS" sheetId="1" r:id="rId1"/>
     <sheet name="RESULTS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t>MODEL</t>
+  </si>
+  <si>
+    <t>TARGET_COLUMN_ID</t>
+  </si>
+  <si>
+    <t>COLUMN_1</t>
+  </si>
+  <si>
+    <t>COLUMN_2</t>
+  </si>
+  <si>
+    <t>COLUMN_3</t>
+  </si>
+  <si>
+    <t>COLUMN_4</t>
+  </si>
+  <si>
+    <t>RATING_COLUMN</t>
+  </si>
+  <si>
+    <t>TARGET_COLUMN</t>
+  </si>
   <si>
     <t>VADER</t>
   </si>
@@ -98,8 +128,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +192,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -208,7 +246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,9 +278,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,6 +330,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -449,56 +523,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -507,117 +610,138 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>276</v>
       </c>
       <c r="C2">
-        <v>0.6249</v>
+        <v>0.62490000000000001</v>
       </c>
       <c r="D2">
-        <v>0.4974916666666666</v>
+        <v>0.49749166666666661</v>
       </c>
       <c r="E2">
-        <v>0.4413948035729602</v>
+        <v>0.44139480357296018</v>
       </c>
       <c r="F2">
-        <v>-0.9762</v>
+        <v>-0.97619999999999996</v>
       </c>
       <c r="G2">
         <v>0.2732</v>
       </c>
       <c r="H2">
-        <v>0.6249</v>
+        <v>0.62490000000000001</v>
       </c>
       <c r="I2">
-        <v>0.8523499999999999</v>
+        <v>0.85234999999999994</v>
       </c>
       <c r="J2">
-        <v>0.9907</v>
+        <v>0.99070000000000003</v>
       </c>
       <c r="K2">
-        <v>0.8188</v>
+        <v>0.81879999999999997</v>
       </c>
       <c r="L2">
-        <v>0.0761</v>
+        <v>7.6100000000000001E-2</v>
       </c>
       <c r="M2">
         <v>0.1051</v>
       </c>
       <c r="N2">
-        <v>0.4413833017401382</v>
+        <v>0.44138330174013818</v>
       </c>
       <c r="O2">
-        <v>1.377116003577516E-14</v>
+        <v>1.3771160035775159E-14</v>
       </c>
       <c r="P2">
-        <v>0.6384982566153495</v>
+        <v>0.63849825661534954</v>
       </c>
       <c r="Q2">
-        <v>5.193686506064902E-33</v>
+        <v>5.1936865060649022E-33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>